<commit_message>
multiple changes to all parts
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>wood_thickness</t>
   </si>
@@ -189,9 +189,6 @@
     <t>frame_foot_z</t>
   </si>
   <si>
-    <t>drawer_z_from_bottom</t>
-  </si>
-  <si>
     <t>end_stop_offset_x</t>
   </si>
   <si>
@@ -283,6 +280,12 @@
   </si>
   <si>
     <t>m5_press_nut_drill</t>
+  </si>
+  <si>
+    <t>drawer_support_overlap</t>
+  </si>
+  <si>
+    <t>drawer_support_from_top</t>
   </si>
 </sst>
 </file>
@@ -621,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,19 +637,19 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1">
         <f>25.4/16</f>
         <v>1.5874999999999999</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <f>9*1.05</f>
@@ -662,7 +665,7 @@
         <v>5.88</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,7 +686,7 @@
         <v>3.1500000000000004</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,18 +706,18 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,18 +736,18 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -757,7 +760,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <v>6.7</v>
@@ -765,24 +768,24 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14">
         <v>4.5</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15">
         <v>6.5</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,7 +836,7 @@
         <v>350</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,7 +847,7 @@
         <v>251</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -855,64 +858,64 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24">
         <f>B21-B64*2</f>
         <v>257.3</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25">
         <f>B81+B26+B1</f>
         <v>110.23750000000001</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27">
         <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,7 +927,7 @@
         <v>334.91250000000002</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -936,64 +939,66 @@
         <v>92.0625</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <f>B84</f>
+        <v>47.467500000000001</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33">
         <f>B44</f>
         <v>251</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34">
         <f>B29</f>
         <v>334.91250000000002</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35">
-        <v>30</v>
+        <f>B84</f>
+        <v>47.467500000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1002,10 +1007,10 @@
       </c>
       <c r="B36">
         <f>B44-B43*2</f>
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,32 +1019,32 @@
       </c>
       <c r="B37">
         <f>B45-B43*2</f>
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1047,11 +1052,11 @@
         <v>14</v>
       </c>
       <c r="B40">
-        <f>B36+66</f>
-        <v>277</v>
+        <f>B36+70</f>
+        <v>271</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,7 +1067,7 @@
         <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,7 +1078,7 @@
         <v>300</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,7 +1086,10 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1093,7 +1101,7 @@
         <v>251</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1105,7 +1113,7 @@
         <v>251</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1113,11 +1121,11 @@
         <v>17</v>
       </c>
       <c r="B46">
-        <f>B36-61</f>
+        <f>B36-51</f>
         <v>150</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,34 +1133,34 @@
         <v>18</v>
       </c>
       <c r="B47">
-        <f>B37-61</f>
+        <f>B37-51</f>
         <v>150</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48">
         <v>25.4</v>
       </c>
       <c r="D48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49">
         <f>B38+B53-B48+5</f>
-        <v>89.6</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,7 +1171,7 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1183,7 @@
         <v>330</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,7 +1194,7 @@
         <v>70</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,23 +1205,23 @@
         <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54">
         <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <f>B46/3</f>
@@ -1222,7 +1230,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>19</v>
@@ -1230,7 +1238,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1238,7 +1246,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>7</v>
@@ -1262,7 +1270,7 @@
         <v>386</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,7 +1281,7 @@
         <v>275</v>
       </c>
       <c r="D61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,7 +1293,7 @@
         <v>661</v>
       </c>
       <c r="D62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,7 +1305,7 @@
         <v>80</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,7 +1317,7 @@
         <v>46.35</v>
       </c>
       <c r="D64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,7 +1328,7 @@
         <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,7 +1459,7 @@
         <v>257.3</v>
       </c>
       <c r="D80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1463,7 +1471,7 @@
         <v>88.65</v>
       </c>
       <c r="D81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1475,41 +1483,52 @@
         <v>278.17500000000001</v>
       </c>
       <c r="D82" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="B83">
-        <f>25</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D83" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B84">
-        <v>60</v>
+        <f>B38+B3+B1</f>
+        <v>47.467500000000001</v>
       </c>
       <c r="D84" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B85">
+        <v>60</v>
+      </c>
+      <c r="D85" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86">
         <v>43</v>
       </c>
-      <c r="D85" t="s">
-        <v>65</v>
+      <c r="D86" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start of day commit
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -16,20 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>wood_thickness</t>
   </si>
   <si>
-    <t>stepper_screw_space</t>
-  </si>
-  <si>
-    <t>stepper_shaft_diameter</t>
-  </si>
-  <si>
-    <t>stepper_body_diameter</t>
-  </si>
-  <si>
     <t>m3_diameter</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>stopper_diameter</t>
   </si>
   <si>
-    <t>z_min_from_center</t>
-  </si>
-  <si>
     <t>linear_bearing_z</t>
   </si>
   <si>
@@ -105,24 +93,9 @@
     <t>window_z</t>
   </si>
   <si>
-    <t>frame_tilt</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
     <t>clear_acrylic</t>
   </si>
   <si>
-    <t>subframe_z</t>
-  </si>
-  <si>
-    <t>subframe_x</t>
-  </si>
-  <si>
-    <t>subframe_y_offset</t>
-  </si>
-  <si>
     <t>laser_y_offset</t>
   </si>
   <si>
@@ -159,9 +132,6 @@
     <t>galvo_frame_z</t>
   </si>
   <si>
-    <t>t_galvo_frame</t>
-  </si>
-  <si>
     <t>galvo_frame_y_offset</t>
   </si>
   <si>
@@ -189,18 +159,9 @@
     <t>frame_foot_z</t>
   </si>
   <si>
-    <t>end_stop_offset_x</t>
-  </si>
-  <si>
     <t>end_stop_spacing</t>
   </si>
   <si>
-    <t>thumb_nut_offset_y</t>
-  </si>
-  <si>
-    <t>thumb_nut_diameter</t>
-  </si>
-  <si>
     <t>m5_brass_insert_drill</t>
   </si>
   <si>
@@ -286,6 +247,27 @@
   </si>
   <si>
     <t>drawer_support_from_top</t>
+  </si>
+  <si>
+    <t>laser_gap</t>
+  </si>
+  <si>
+    <t>frame_screw_from_center</t>
+  </si>
+  <si>
+    <t>galvo_frame_y</t>
+  </si>
+  <si>
+    <t>frame_magnet_offset</t>
+  </si>
+  <si>
+    <t>magnet_z</t>
+  </si>
+  <si>
+    <t>drawer_screw_z</t>
+  </si>
+  <si>
+    <t>drawer_screw_from_center</t>
   </si>
 </sst>
 </file>
@@ -624,32 +606,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B1">
         <f>25.4/16</f>
         <v>1.5874999999999999</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <f>9*1.05</f>
@@ -658,19 +640,19 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <f>5.6*1.05</f>
         <v>5.88</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <f>3*1.05</f>
@@ -679,14 +661,14 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <f>3*1.05</f>
         <v>3.1500000000000004</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,29 +682,29 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -730,29 +712,29 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -760,7 +742,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>6.7</v>
@@ -768,48 +750,54 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>4.5</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <v>6.5</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>28</v>
+        <v>350</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,279 +805,288 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>251</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>12</v>
       </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B21">
-        <v>350</v>
+        <f>B18-B57*2</f>
+        <v>257.3</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="B22">
-        <v>251</v>
+        <f>B74+B23+B1</f>
+        <v>110.23750000000001</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B24">
-        <f>B21-B64*2</f>
-        <v>257.3</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B25">
-        <f>B81+B26+B1</f>
-        <v>110.23750000000001</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>20</v>
+        <f>B53-B57-B4-B1</f>
+        <v>333.91250000000002</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B27">
-        <v>80</v>
+        <f>B74-B1+B29</f>
+        <v>92.0625</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <f>B77</f>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B29">
-        <f>B60-B64-B4-B1</f>
-        <v>334.91250000000002</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B30">
-        <f>B81-B1+B32</f>
-        <v>92.0625</v>
+        <f>B41</f>
+        <v>251</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B31">
-        <f>B84</f>
-        <v>47.467500000000001</v>
+        <f>B26</f>
+        <v>333.91250000000002</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <f>B77</f>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B33">
-        <f>B44</f>
-        <v>251</v>
+        <f>B41-B40*2</f>
+        <v>201</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="B34">
-        <f>B29</f>
-        <v>334.91250000000002</v>
+        <f>B42-B40*2</f>
+        <v>201</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B35">
-        <f>B84</f>
-        <v>47.467500000000001</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B36">
-        <f>B44-B43*2</f>
-        <v>201</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37">
-        <f>B45-B43*2</f>
-        <v>201</v>
+        <f>B33+70</f>
+        <v>271</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="B38">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B40">
-        <f>B36+70</f>
-        <v>271</v>
+        <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B41">
-        <v>400</v>
+        <f>B42</f>
+        <v>251</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B42">
-        <v>300</v>
+        <f>B19</f>
+        <v>251</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B43">
-        <v>25</v>
+        <f>B33-51</f>
+        <v>150</v>
       </c>
       <c r="D43" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,238 +1094,243 @@
         <v>15</v>
       </c>
       <c r="B44">
-        <f>B45</f>
-        <v>251</v>
+        <f>B34-51</f>
+        <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B45">
-        <f>B22</f>
-        <v>251</v>
+        <v>25</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B46">
-        <f>B36-51</f>
-        <v>150</v>
+        <f>B35+B50-B45+5</f>
+        <v>80</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B47">
-        <f>B37-51</f>
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B48">
-        <v>25.4</v>
+        <f>B18-20</f>
+        <v>330</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="B49">
-        <f>B38+B53-B48+5</f>
-        <v>79.599999999999994</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B50">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B51">
-        <f>B21-20</f>
-        <v>330</v>
+        <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B52">
-        <v>70</v>
-      </c>
-      <c r="D52" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B53">
-        <v>60</v>
+        <f>FLOOR(B38-10-B1*2,5)</f>
+        <v>385</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="B54">
-        <v>12</v>
+        <f>275</f>
+        <v>275</v>
       </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B55">
-        <f>B46/3</f>
-        <v>50</v>
+        <f>B54+B53+B1</f>
+        <v>661.58749999999998</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <f>B49+10</f>
+        <v>80</v>
+      </c>
+      <c r="D56" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <f>(B18-B41)/2-B5</f>
+        <v>46.35</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="D58" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="B59">
-        <f>B51/2-50</f>
-        <v>115</v>
+        <v>45</v>
+      </c>
+      <c r="D59" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B60">
-        <f>FLOOR(B41-10-B1*2,1)</f>
-        <v>386</v>
+        <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B61">
-        <v>275</v>
+        <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B62">
-        <f>B61+B60</f>
-        <v>661</v>
-      </c>
-      <c r="D62" t="s">
-        <v>64</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B63">
-        <f>B52+10</f>
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B64">
-        <f>(B21-B44)/2-B5</f>
-        <v>46.35</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B65">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D65" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,199 +1338,181 @@
         <v>29</v>
       </c>
       <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
-        <v>30</v>
+        <v>75</v>
+      </c>
+      <c r="D66" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B67">
-        <f>B21/2+20</f>
-        <v>195</v>
+        <v>30</v>
+      </c>
+      <c r="D67" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="B68">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B69">
-        <v>27.5</v>
+        <v>66</v>
+      </c>
+      <c r="D69" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B70">
-        <v>19.399999999999999</v>
+        <v>20</v>
+      </c>
+      <c r="D70" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>65</v>
+      </c>
+      <c r="D71" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B72">
-        <v>55</v>
+        <f>27.5</f>
+        <v>27.5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B73">
-        <v>35</v>
+        <f>B41+B4*2</f>
+        <v>257.3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B74">
-        <f>(B68-51)*2</f>
-        <v>18</v>
+        <f>(B19-B56)/2+B4</f>
+        <v>88.65</v>
+      </c>
+      <c r="D74" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B75">
-        <v>24</v>
+        <f>B54+B1*2</f>
+        <v>278.17500000000001</v>
+      </c>
+      <c r="D75" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B76">
-        <f>B6</f>
-        <v>6.7200000000000006</v>
+        <v>40</v>
+      </c>
+      <c r="D76" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B77">
-        <v>66</v>
+        <f>CEILING(B35+B3+B1,1)</f>
+        <v>48</v>
+      </c>
+      <c r="D77" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B78">
-        <v>65</v>
+        <f>CEILING(B57+B59+25,1)</f>
+        <v>117</v>
+      </c>
+      <c r="D78" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B79">
-        <f>27.5</f>
-        <v>27.5</v>
+        <v>50</v>
+      </c>
+      <c r="D79" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B80">
-        <f>B44+B4*2</f>
-        <v>257.3</v>
+        <v>60</v>
       </c>
       <c r="D80" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B81">
-        <f>(B22-B63)/2+B4</f>
-        <v>88.65</v>
+        <v>43</v>
       </c>
       <c r="D81" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>55</v>
-      </c>
-      <c r="B82">
-        <f>B61+B1*2</f>
-        <v>278.17500000000001</v>
-      </c>
-      <c r="D82" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>88</v>
-      </c>
-      <c r="B83">
-        <v>40</v>
-      </c>
-      <c r="D83" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84">
-        <f>B38+B3+B1</f>
-        <v>47.467500000000001</v>
-      </c>
-      <c r="D84" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>71</v>
-      </c>
-      <c r="B85">
-        <v>60</v>
-      </c>
-      <c r="D85" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86">
-        <v>43</v>
-      </c>
-      <c r="D86" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added drawer holes for screw and magnets
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
   <si>
     <t>wood_thickness</t>
   </si>
@@ -159,9 +159,6 @@
     <t>frame_foot_z</t>
   </si>
   <si>
-    <t>end_stop_spacing</t>
-  </si>
-  <si>
     <t>m5_brass_insert_drill</t>
   </si>
   <si>
@@ -268,6 +265,18 @@
   </si>
   <si>
     <t>drawer_screw_from_center</t>
+  </si>
+  <si>
+    <t>frame_face_y</t>
+  </si>
+  <si>
+    <t>magnet_screw_spacing</t>
+  </si>
+  <si>
+    <t>magnet_screw_from_edge</t>
+  </si>
+  <si>
+    <t>switch_spacing</t>
   </si>
 </sst>
 </file>
@@ -606,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,19 +628,19 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1">
         <f>25.4/16</f>
         <v>1.5874999999999999</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <f>9*1.05</f>
@@ -647,7 +656,7 @@
         <v>5.88</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,7 +677,7 @@
         <v>3.1500000000000004</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,18 +697,18 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -718,18 +727,18 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,7 +751,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>6.7</v>
@@ -750,24 +759,24 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14">
         <v>4.5</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15">
         <v>6.5</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,7 +806,7 @@
         <v>350</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,7 +817,7 @@
         <v>251</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,64 +828,64 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21">
-        <f>B18-B57*2</f>
+        <f>B18-B58*2</f>
         <v>257.3</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22">
-        <f>B74+B23+B1</f>
+        <f>B77+B23+B1</f>
         <v>110.23750000000001</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23">
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,11 +893,11 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <f>B53-B57-B4-B1</f>
+        <f>B53-B58-B4-B1</f>
         <v>333.91250000000002</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -896,70 +905,70 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <f>B74-B1+B29</f>
+        <f>B77-B1+B29</f>
         <v>92.0625</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28">
-        <f>B77</f>
+        <f>B80</f>
         <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <f>B41</f>
         <v>251</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31">
         <f>B26</f>
         <v>333.91250000000002</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32">
-        <f>B77</f>
+        <f>B80</f>
         <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,7 +980,7 @@
         <v>201</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -983,29 +992,29 @@
         <v>201</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35">
         <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36">
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1017,7 +1026,7 @@
         <v>271</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1028,7 +1037,7 @@
         <v>400</v>
       </c>
       <c r="D38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1039,7 +1048,7 @@
         <v>300</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,7 +1059,7 @@
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,7 +1071,7 @@
         <v>251</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,7 +1083,7 @@
         <v>251</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,7 +1095,7 @@
         <v>150</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,30 +1107,30 @@
         <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45">
         <v>25</v>
       </c>
       <c r="D45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46">
         <f>B35+B50-B45+5</f>
         <v>80</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1144,7 +1153,7 @@
         <v>330</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1155,7 +1164,7 @@
         <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1166,26 +1175,29 @@
         <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51">
         <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B52">
         <v>19</v>
+      </c>
+      <c r="D52" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,7 +1209,7 @@
         <v>385</v>
       </c>
       <c r="D53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1209,7 +1221,7 @@
         <v>275</v>
       </c>
       <c r="D54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,7 +1233,7 @@
         <v>661.58749999999998</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1233,286 +1245,323 @@
         <v>80</v>
       </c>
       <c r="D56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57">
+        <f>CEILING(B56/2+B1*2,1)</f>
+        <v>44</v>
+      </c>
+      <c r="D57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>33</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <f>(B18-B41)/2-B5</f>
         <v>46.35</v>
       </c>
-      <c r="D57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58">
-        <v>20</v>
-      </c>
       <c r="D58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B59">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B60">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D60" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B61">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="B62">
-        <v>19.399999999999999</v>
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B63">
         <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B64">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B65">
-        <v>15</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D65" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B66">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B67">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B69">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="B70">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B71">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72">
+        <v>66</v>
+      </c>
+      <c r="D72" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73">
+        <v>20</v>
+      </c>
+      <c r="D73" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>37</v>
+      </c>
+      <c r="B74">
+        <v>65</v>
+      </c>
+      <c r="D74" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>38</v>
       </c>
-      <c r="B72">
+      <c r="B75">
         <f>27.5</f>
         <v>27.5</v>
       </c>
-      <c r="D72" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="D75" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>43</v>
       </c>
-      <c r="B73">
+      <c r="B76">
         <f>B41+B4*2</f>
         <v>257.3</v>
       </c>
-      <c r="D73" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="D76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>44</v>
       </c>
-      <c r="B74">
+      <c r="B77">
         <f>(B19-B56)/2+B4</f>
         <v>88.65</v>
       </c>
-      <c r="D74" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="D77" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>45</v>
       </c>
-      <c r="B75">
+      <c r="B78">
         <f>B54+B1*2</f>
         <v>278.17500000000001</v>
       </c>
-      <c r="D75" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="D78" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79">
+        <v>40</v>
+      </c>
+      <c r="D79" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>75</v>
       </c>
-      <c r="B76">
-        <v>40</v>
-      </c>
-      <c r="D76" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>76</v>
-      </c>
-      <c r="B77">
+      <c r="B80">
         <f>CEILING(B35+B3+B1,1)</f>
         <v>48</v>
       </c>
-      <c r="D77" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78">
-        <f>CEILING(B57+B59+25,1)</f>
-        <v>117</v>
-      </c>
-      <c r="D78" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79">
-        <v>50</v>
-      </c>
-      <c r="D79" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>58</v>
-      </c>
-      <c r="B80">
-        <v>60</v>
-      </c>
       <c r="D80" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B81">
+        <f>CEILING(B58+B60+25,1)</f>
+        <v>117</v>
+      </c>
+      <c r="D81" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>50</v>
+      </c>
+      <c r="D82" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83">
+        <v>60</v>
+      </c>
+      <c r="D83" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84">
         <v>43</v>
       </c>
-      <c r="D81" t="s">
-        <v>51</v>
+      <c r="D84" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated params and drawer locking
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,8 +848,8 @@
         <v>62</v>
       </c>
       <c r="B22">
-        <f>B77+B23+B1</f>
-        <v>110.23750000000001</v>
+        <f>B77+B23+B57-B56/2-B1</f>
+        <v>111.0625</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
@@ -1257,7 +1257,7 @@
         <v>44</v>
       </c>
       <c r="D57" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,7 +1288,7 @@
         <v>80</v>
       </c>
       <c r="B60">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D60" t="s">
         <v>56</v>
@@ -1524,8 +1524,8 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <f>CEILING(B58+B60+25,1)</f>
-        <v>117</v>
+        <f>FLOOR(B78-B80-B79-B60,1)</f>
+        <v>140</v>
       </c>
       <c r="D81" t="s">
         <v>56</v>
@@ -1536,7 +1536,8 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>50</v>
+        <f>B57+B62</f>
+        <v>54</v>
       </c>
       <c r="D82" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
First stab at 2d cad files
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bug fixes, changed how bed connects to crane
New mounting method allows for some Z adjust
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,8 +1132,8 @@
         <v>59</v>
       </c>
       <c r="B46">
-        <f>B35+B50-B45+5</f>
-        <v>80</v>
+        <f>B35+B50/2-B45+5</f>
+        <v>50</v>
       </c>
       <c r="D46" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
First completion of v1.2
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fully updated 2D drawings for V1.2
</commit_message>
<xml_diff>
--- a/laserresin4.xlsx
+++ b/laserresin4.xlsx
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1589,7 @@
         <v>37</v>
       </c>
       <c r="B84">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="D84" t="s">
         <v>50</v>

</xml_diff>